<commit_message>
chore: import template column changes
</commit_message>
<xml_diff>
--- a/public/assets/static/template/template-dokumen.xlsx
+++ b/public/assets/static/template/template-dokumen.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akmal\Latihan Pemograman\laravel\sirepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B20D250-59A5-40FD-9AE2-E4177085BC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6EF2A73F-2D15-48AC-8CE8-41A68F311669}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Jenis Dokumen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Judul</t>
   </si>
@@ -37,43 +35,25 @@
     <t>Penulis</t>
   </si>
   <si>
-    <t xml:space="preserve">Penguji </t>
+    <t>Pembimbing</t>
+  </si>
+  <si>
+    <t>Penguji</t>
+  </si>
+  <si>
+    <t>Jenis</t>
   </si>
   <si>
     <t>Tahun</t>
   </si>
   <si>
     <t>Keyword</t>
-  </si>
-  <si>
-    <t>Pembimbing</t>
-  </si>
-  <si>
-    <t>Proyek2</t>
-  </si>
-  <si>
-    <t>PKL</t>
-  </si>
-  <si>
-    <t>jenis_id</t>
-  </si>
-  <si>
-    <t>Proyek1</t>
-  </si>
-  <si>
-    <t>Tugas Akhir</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Jenis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,20 +83,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,113 +398,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6991E78-2052-4FDD-9D66-B112CC37D746}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231D3A5D-C8C5-45A2-AE67-C577DC0EB5F7}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>